<commit_message>
Update: Will now print out a basic schedule for a 16 week Marathon training plan.
</commit_message>
<xml_diff>
--- a/test-equations.xlsx
+++ b/test-equations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b44cf06eb83b68b2/Learn With Leon/Projects/Training Plan Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59BE773F-51B7-4827-B2B6-88B9FB7B9292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{59BE773F-51B7-4827-B2B6-88B9FB7B9292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84C10E99-D2E3-4894-89C9-D42C65BB6B94}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CA9D64BF-6409-48B1-8673-59E57B6FE98B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CA9D64BF-6409-48B1-8673-59E57B6FE98B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Week</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>goalDistance</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
@@ -97,10 +106,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,18 +431,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A4E57A-C1BD-4637-9CB7-19DB73185137}">
-  <dimension ref="E8:K27"/>
+  <dimension ref="E8:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="U18" sqref="U18:W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
@@ -435,7 +450,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
@@ -443,15 +458,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
@@ -461,153 +479,296 @@
       <c r="I11" t="s">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="J11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <f>K13-2</f>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <f>K12/maxMileage</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q12">
+        <f>Q13-2</f>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I13">
         <v>1</v>
       </c>
-      <c r="K13">
-        <f>K14-2</f>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2">
+        <v>28</v>
+      </c>
+      <c r="L13">
+        <f>K13/maxMileage</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q13">
+        <f>Q14-2</f>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I14">
         <v>2</v>
       </c>
-      <c r="K14">
-        <f>K15-2</f>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
+        <v>33</v>
+      </c>
+      <c r="L14">
+        <f>K14/maxMileage</f>
+        <v>0.66</v>
+      </c>
+      <c r="Q14">
+        <f>Q15-2</f>
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I15">
         <v>3</v>
       </c>
-      <c r="K15">
-        <f>K16-2</f>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2">
+        <v>37</v>
+      </c>
+      <c r="L15">
+        <f>K15/maxMileage</f>
+        <v>0.74</v>
+      </c>
+      <c r="Q15">
+        <f>Q16-2</f>
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I16">
         <v>4</v>
       </c>
-      <c r="K16">
-        <f>K18-1</f>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2">
+        <v>40</v>
+      </c>
+      <c r="L16">
+        <f>K16/maxMileage</f>
+        <v>0.8</v>
+      </c>
+      <c r="Q16">
+        <f>Q18-1</f>
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I17">
         <v>5</v>
       </c>
-      <c r="K17">
-        <f>K19</f>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2">
+        <v>44</v>
+      </c>
+      <c r="L17">
+        <f>K17/maxMileage</f>
+        <v>0.88</v>
+      </c>
+      <c r="Q17">
+        <f>Q19</f>
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I18">
         <v>6</v>
       </c>
-      <c r="K18">
-        <f>K20-1</f>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2">
+        <v>48</v>
+      </c>
+      <c r="L18">
+        <f>K18/maxMileage</f>
+        <v>0.96</v>
+      </c>
+      <c r="Q18">
+        <f>Q20-1</f>
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I19">
         <v>7</v>
       </c>
-      <c r="K19">
-        <f>K21-1</f>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2">
+        <v>40</v>
+      </c>
+      <c r="L19">
+        <f>K19/maxMileage</f>
+        <v>0.8</v>
+      </c>
+      <c r="Q19">
+        <f>Q21-1</f>
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I20">
         <v>8</v>
       </c>
-      <c r="K20">
+      <c r="J20" s="2">
+        <f>maxMileage</f>
+        <v>50</v>
+      </c>
+      <c r="K20" s="2">
+        <v>50</v>
+      </c>
+      <c r="L20">
+        <f>K20/maxMileage</f>
+        <v>1</v>
+      </c>
+      <c r="Q20">
         <f>maxLR</f>
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I21">
         <v>9</v>
       </c>
-      <c r="K21">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2">
+        <v>42</v>
+      </c>
+      <c r="L21">
+        <f>K21/maxMileage</f>
+        <v>0.84</v>
+      </c>
+      <c r="Q21">
         <f>maxLR * 0.85</f>
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I22">
         <v>10</v>
       </c>
-      <c r="K22">
+      <c r="J22" s="2">
+        <f>maxMileage</f>
+        <v>50</v>
+      </c>
+      <c r="K22" s="2">
+        <v>50</v>
+      </c>
+      <c r="L22">
+        <f>K22/maxMileage</f>
+        <v>1</v>
+      </c>
+      <c r="Q22">
         <f>maxLR</f>
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I23">
         <v>11</v>
       </c>
-      <c r="K23">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2">
+        <v>42</v>
+      </c>
+      <c r="L23">
+        <f>K23/maxMileage</f>
+        <v>0.84</v>
+      </c>
+      <c r="Q23">
         <f>maxLR * 0.85</f>
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I24">
         <v>12</v>
       </c>
-      <c r="K24">
+      <c r="J24" s="2">
+        <f>maxMileage</f>
+        <v>50</v>
+      </c>
+      <c r="K24" s="2">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <f>K24/maxMileage</f>
+        <v>1</v>
+      </c>
+      <c r="Q24">
         <f>maxLR</f>
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I25">
         <v>13</v>
       </c>
-      <c r="K25">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2">
+        <v>40</v>
+      </c>
+      <c r="L25">
+        <f>K25/maxMileage</f>
+        <v>0.8</v>
+      </c>
+      <c r="Q25">
         <f>maxLR * 0.8</f>
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26">
         <v>14</v>
       </c>
-      <c r="K26">
+      <c r="J26" s="2"/>
+      <c r="K26" s="2">
+        <v>30</v>
+      </c>
+      <c r="L26">
+        <f>K26/maxMileage</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q26">
         <f>maxLR*0.6</f>
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I27">
         <v>15</v>
       </c>
-      <c r="K27">
+      <c r="J27" s="2"/>
+      <c r="K27" s="2">
+        <v>20</v>
+      </c>
+      <c r="L27">
+        <f>K27/maxMileage</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q27">
         <f>goalDistance</f>
         <v>26.2</v>
       </c>

</xml_diff>